<commit_message>
some results diagrams added
</commit_message>
<xml_diff>
--- a/SolarHeatingSystem/summary.xlsx
+++ b/SolarHeatingSystem/summary.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\AI_DATA\ModelicaLibraries\modelica-annex60_BuildingDesign\SolarHeatingSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nytschgeusen\VirtualBox\modelica-annex60_BuildingDesign\SolarHeatingSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,11 +13,12 @@
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="detailedOutput" localSheetId="0">Tabelle1!$A$17:$B$24</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>City</t>
   </si>
@@ -64,12 +65,6 @@
   </si>
   <si>
     <t>costfunction in €</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>San Francisco</t>
   </si>
   <si>
     <t>costInsulation</t>
@@ -125,6 +120,30 @@
   <si>
     <t>execution time in GenOpt</t>
   </si>
+  <si>
+    <t>Chicago (pen = 500 €, EP = 0.08 €)</t>
+  </si>
+  <si>
+    <t>Chicago (pen = 500 €, EP = 0.16 €)</t>
+  </si>
+  <si>
+    <t>Chicago (pen = 1500 €, EP = 0.08 €)</t>
+  </si>
+  <si>
+    <t>Chicago (pen = 1500 €, EP = 0.16 €)</t>
+  </si>
+  <si>
+    <t>San Francisco (pen = 500 €, EP = 0.08 €)</t>
+  </si>
+  <si>
+    <t>San Francisco (pen = 500 €, EP = 0.16 €)</t>
+  </si>
+  <si>
+    <t>San Francisco (pen = 1500 €, EP = 0.08 €)</t>
+  </si>
+  <si>
+    <t>San Francisco (pen = 1500 €, EP = 0.16 €)</t>
+  </si>
 </sst>
 </file>
 
@@ -179,6 +198,2830 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.000" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Chicago (pen = 500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chicago (pen = 500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chicago (pen = 1500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Chicago (pen = 1500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>San Francisco (pen = 500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>San Francisco (pen = 500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>San Francisco (pen = 1500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>San Francisco (pen = 1500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$F$2:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.1575</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22875000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26250000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7500000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10125000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.375E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7083-437C-9A29-715487AE12A2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="962635711"/>
+        <c:axId val="904423263"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="962635711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="904423263"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="904423263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200"/>
+                  <a:t>thickness insulation im m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="962635711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Chicago (pen = 500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chicago (pen = 500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chicago (pen = 1500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Chicago (pen = 1500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>San Francisco (pen = 500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>San Francisco (pen = 500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>San Francisco (pen = 1500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>San Francisco (pen = 1500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-65A7-4585-9EA0-F1760660C0BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="962635711"/>
+        <c:axId val="904423263"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="962635711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="904423263"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="904423263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200"/>
+                  <a:t>Volume solar storage in m3</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="962635711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Tabelle1!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Chicago (pen = 500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chicago (pen = 500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Chicago (pen = 1500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Chicago (pen = 1500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>San Francisco (pen = 500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>San Francisco (pen = 500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>San Francisco (pen = 1500 €, EP = 0.08 €)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>San Francisco (pen = 1500 €, EP = 0.16 €)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$G$2:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>6.7106483267813405E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.6497338308173499E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17970492756244999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.218069945947062</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.47763140318313302</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.48689051543659201</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.50716729335481003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.49980572852288002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ADBE-4D38-AA79-C45C00E4E746}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="962635711"/>
+        <c:axId val="904423263"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="962635711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="904423263"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="904423263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1200"/>
+                  <a:t>Solar coverage rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="962635711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -261,23 +3104,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -313,23 +3139,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,13 +3293,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
@@ -536,39 +3345,39 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>24</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>25</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>0.08</v>
@@ -626,7 +3435,7 @@
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>0.16</v>
@@ -683,8 +3492,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
+      <c r="A4" t="s">
+        <v>28</v>
       </c>
       <c r="B4" s="1">
         <v>0.08</v>
@@ -741,8 +3550,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
+      <c r="A5" t="s">
+        <v>29</v>
       </c>
       <c r="B5" s="1">
         <v>0.16</v>
@@ -799,8 +3608,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
+      <c r="A6" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="1">
         <v>0.08</v>
@@ -858,7 +3667,7 @@
     </row>
     <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B7">
         <v>0.16</v>
@@ -915,8 +3724,8 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>9</v>
+      <c r="A8" t="s">
+        <v>32</v>
       </c>
       <c r="B8" s="1">
         <v>0.08</v>
@@ -974,7 +3783,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="B9">
         <v>0.16</v>
@@ -1032,12 +3841,12 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>312.49644699049497</v>
@@ -1045,7 +3854,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -1053,7 +3862,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>1099.6658933333299</v>
@@ -1061,7 +3870,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B20">
         <v>16888968264.643801</v>
@@ -1069,7 +3878,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>21599078046.820301</v>
@@ -1085,7 +3894,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23">
         <v>750.62081176194602</v>
@@ -1093,7 +3902,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24">
         <v>422.89508107940497</v>
@@ -1106,5 +3915,18 @@
     <sortCondition ref="B2:B9"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding results from new optimization, model writes data into output file now
</commit_message>
<xml_diff>
--- a/SolarHeatingSystem/summary.xlsx
+++ b/SolarHeatingSystem/summary.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nytschgeusen\VirtualBox\modelica-annex60_BuildingDesign\SolarHeatingSystem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\AI_DATA\ModelicaLibraries\modelica-annex60_BuildingDesign\SolarHeatingSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35160" windowHeight="13875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35160" windowHeight="13875" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="altes Zeug" sheetId="1" r:id="rId1"/>
+    <sheet name="neue Optimierung" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="detailedOutput" localSheetId="0">Tabelle1!$A$17:$B$24</definedName>
+    <definedName name="dataOutput" localSheetId="1">'neue Optimierung'!$A$18:$B$25</definedName>
+    <definedName name="detailedOutput" localSheetId="0">'altes Zeug'!$A$17:$B$24</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,15 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="detailedOutput" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="1" name="dataOutput" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="C:\Users\alexa\AI_DATA\ModelicaLibraries\modelica-annex60_BuildingDesign\SolarHeatingSystem\dataOutput.txt" tab="0" comma="1">
+      <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="detailedOutput" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="C:\Users\alexa\AI_DATA\ModelicaLibraries\modelica-annex60_BuildingDesign\SolarHeatingSystem\detailedOutput.txt" comma="1">
       <textFields count="2">
         <textField/>
@@ -41,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>City</t>
   </si>
@@ -144,6 +153,39 @@
   <si>
     <t>San Francisco (pen = 1500 €, EP = 0.16 €)</t>
   </si>
+  <si>
+    <t>Chicago (pen = 0 €, EP = 0.08 €)</t>
+  </si>
+  <si>
+    <t>San Francisco (pen = 0 €, EP = 0.08 €)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">costStorage = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">costCollector = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">costInsulation = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">heaterEnergy = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">radiatorEnergy = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">solarfraction = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">costHeaterEnergy = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">costPenalty = </t>
+  </si>
+  <si>
+    <t>Imported fields</t>
+  </si>
 </sst>
 </file>
 
@@ -187,8 +229,36 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -274,7 +344,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -295,7 +364,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$9</c:f>
+              <c:f>'altes Zeug'!$A$2:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -327,7 +396,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$F$2:$F$9</c:f>
+              <c:f>'altes Zeug'!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -475,7 +544,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -659,7 +727,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -680,7 +747,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$9</c:f>
+              <c:f>'altes Zeug'!$A$2:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -712,7 +779,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$2:$D$9</c:f>
+              <c:f>'altes Zeug'!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -860,7 +927,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1006,7 +1072,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$9</c:f>
+              <c:f>'altes Zeug'!$A$2:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -1038,7 +1104,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$G$2:$G$9</c:f>
+              <c:f>'altes Zeug'!$G$2:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1186,7 +1252,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3025,7 +3090,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="detailedOutput" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="detailedOutput" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dataOutput" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3104,6 +3173,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3139,6 +3225,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3293,8 +3396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="K77" sqref="K77"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3921,12 +4024,392 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>0.08</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3.5</v>
+      </c>
+      <c r="F2">
+        <v>0.15375</v>
+      </c>
+      <c r="G2">
+        <v>8.4562332555727607E-2</v>
+      </c>
+      <c r="H2">
+        <v>1572.73</v>
+      </c>
+      <c r="I2">
+        <v>82.490499999999898</v>
+      </c>
+      <c r="J2">
+        <v>35</v>
+      </c>
+      <c r="K2">
+        <v>907.34462133333295</v>
+      </c>
+      <c r="L2">
+        <v>547.89584913244005</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>24655313210.959801</v>
+      </c>
+      <c r="O2">
+        <v>26932814857.610901</v>
+      </c>
+      <c r="P2">
+        <f>N2/3600/1000</f>
+        <v>6848.6981141554998</v>
+      </c>
+      <c r="Q2">
+        <f>O2/3600/1000</f>
+        <v>7481.3374604474729</v>
+      </c>
+      <c r="R2" s="2">
+        <v>3.1655092592592596E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>0.08</v>
+      </c>
+      <c r="C3">
+        <v>1500</v>
+      </c>
+      <c r="D3">
+        <v>29.5</v>
+      </c>
+      <c r="E3">
+        <v>9.5</v>
+      </c>
+      <c r="F3">
+        <v>0.19875000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.50044828993364199</v>
+      </c>
+      <c r="H3">
+        <v>1856.28</v>
+      </c>
+      <c r="I3">
+        <v>506.09090957839402</v>
+      </c>
+      <c r="J3">
+        <v>95</v>
+      </c>
+      <c r="K3">
+        <v>986.92583733333299</v>
+      </c>
+      <c r="L3">
+        <v>268.26218291322601</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>12071798231.0952</v>
+      </c>
+      <c r="O3">
+        <v>24165262550.080399</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="0">N3/3600/1000</f>
+        <v>3353.2772864153335</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q5" si="1">O3/3600/1000</f>
+        <v>6712.5729305778877</v>
+      </c>
+      <c r="R3" s="2">
+        <v>3.5428240740740739E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>0.08</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>6.3750000000000001E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.196343803338515</v>
+      </c>
+      <c r="H4">
+        <v>905.79</v>
+      </c>
+      <c r="I4">
+        <v>82.490499999999898</v>
+      </c>
+      <c r="J4">
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>748.18218933333299</v>
+      </c>
+      <c r="L4">
+        <v>65.120459327122404</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>2930420669.7205</v>
+      </c>
+      <c r="O4">
+        <v>3646361070.6841302</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>814.00574158902782</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>1012.8780751900362</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1.8217592592592594E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>0.08</v>
+      </c>
+      <c r="C5">
+        <v>1500</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>6.5</v>
+      </c>
+      <c r="F5">
+        <v>0.06</v>
+      </c>
+      <c r="G5">
+        <v>0.50621882178789102</v>
+      </c>
+      <c r="H5">
+        <v>932.78</v>
+      </c>
+      <c r="I5">
+        <v>82.490499999999898</v>
+      </c>
+      <c r="J5">
+        <v>65</v>
+      </c>
+      <c r="K5">
+        <v>741.55042133333302</v>
+      </c>
+      <c r="L5">
+        <v>43.742639485386903</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1968418776.8424101</v>
+      </c>
+      <c r="O5">
+        <v>3986419215.02495</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>546.78299356733612</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>1107.3386708402638</v>
+      </c>
+      <c r="R5" s="2">
+        <v>1.7650462962962962E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>82.490499999999898</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20">
+        <v>741.55042133333302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21">
+        <v>1968418776.8424101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22">
+        <v>3986419215.02495</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23">
+        <v>0.50621882178789102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24">
+        <v>43.742639485386903</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>